<commit_message>
Added Visualisation Tool components
Added webpage files and changed a few files in the appendices
</commit_message>
<xml_diff>
--- a/Appendices/A - Systematic Review/Systemic Review Articles.xlsx
+++ b/Appendices/A - Systematic Review/Systemic Review Articles.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\janfo\Desktop\Final Year Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\janfo\Desktop\Final Year Project\2.) Systematic Review\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A37874F-32AD-462F-AE8A-81231426E4CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D01811C8-4FD0-4973-BD5F-3536FDA4EEF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{CC596862-8245-40C9-B98C-A2A16BAA5A14}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="3" xr2:uid="{CC596862-8245-40C9-B98C-A2A16BAA5A14}"/>
   </bookViews>
   <sheets>
     <sheet name="ACM" sheetId="2" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529" uniqueCount="347">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="340">
   <si>
     <t>Title</t>
   </si>
@@ -938,15 +938,9 @@
     <t>Scopus</t>
   </si>
   <si>
-    <t>✓</t>
-  </si>
-  <si>
     <t>Paper ID</t>
   </si>
   <si>
-    <t>Chosen?</t>
-  </si>
-  <si>
     <t>https://dl-acm-org.ejournals.um.edu.mt/doi/10.1145/3387166</t>
   </si>
   <si>
@@ -977,21 +971,6 @@
     <t>https://dl-acm-org.ejournals.um.edu.mt/doi/10.1145/3436996</t>
   </si>
   <si>
-    <t>https://dl-acm-org.ejournals.um.edu.mt/doi/10.1145/3555578</t>
-  </si>
-  <si>
-    <t>https://dl-acm-org.ejournals.um.edu.mt/doi/10.1145/3564752</t>
-  </si>
-  <si>
-    <t>https://dl-acm-org.ejournals.um.edu.mt/doi/10.1145/3557891</t>
-  </si>
-  <si>
-    <t>https://dl-acm-org.ejournals.um.edu.mt/doi/10.5555/3648699.3648956</t>
-  </si>
-  <si>
-    <t>https://dl-acm-org.ejournals.um.edu.mt/doi/10.1145/3485062</t>
-  </si>
-  <si>
     <t>https://www.proquest.com/compscijour/docview/2492793919/580ADEAA30A04A0BPQ/42?accountid=27934</t>
   </si>
   <si>
@@ -1022,21 +1001,6 @@
     <t>https://www.proquest.com/compscijour/docview/2492793424/580ADEAA30A04A0BPQ/50?accountid=27934</t>
   </si>
   <si>
-    <t>https://www.proquest.com/compscijour/docview/2576123304/580ADEAA30A04A0BPQ/52?accountid=27934</t>
-  </si>
-  <si>
-    <t>https://www.proquest.com/compscijour/docview/2671813662/580ADEAA30A04A0BPQ/56?accountid=27934</t>
-  </si>
-  <si>
-    <t>https://www.proquest.com/compscijour/docview/2734831335/580ADEAA30A04A0BPQ/38?accountid=27934</t>
-  </si>
-  <si>
-    <t>https://www.proquest.com/compscijour/docview/2492793730/580ADEAA30A04A0BPQ/62?accountid=27934</t>
-  </si>
-  <si>
-    <t>https://www.proquest.com/compscijour/docview/2628403733/580ADEAA30A04A0BPQ/63?accountid=27934</t>
-  </si>
-  <si>
     <t>https://www.scopus.com/record/display.uri?eid=2-s2.0-85122031869&amp;origin=resultslist&amp;sort=r-f&amp;src=s&amp;sid=9a6079508c310b83b4cde54a2285d13f&amp;sot=b&amp;sdt=cl&amp;cluster=scosubtype%2C%22ar%22%2Ct%2Bscopubstage%2C%22final%22%2Ct%2Bscolang%2C%22English%22%2Ct%2Bscosrctype%2C%22j%22%2Ct%2Bscoexactkeywords%2C%22Ethics%22%2Ct&amp;s=%28TITLE%28AI+OR+Artificial+Intelligence+OR+artificial+intelligence+OR+ARTIFICIAL+INTELLIGENCE+OR+Artificial%E2%80%90Intelligence+OR+artificial%E2%80%90intelligence+OR+ARTIFICIAL%E2%80%90INTELLIGENCE%29+AND+TITLE-ABS-KEY%28ethic*+OR+Ethic*+OR+ETHIC*%29+AND+TITLE-ABS-KEY%28%28education+OR+Education+OR+EDUCATION%29+OR+%28healthcare+OR+Healthcare+OR+HEALTHCARE%29+OR+%28transportation+OR+Transportation+OR+TRANSPORTATION%29+OR+%28finance+OR+Finance+OR+FINANCE%29+OR+%28retail+OR+Retail+OR+RETAIL%29+OR+%28manufacturing+OR+Manufacturing+OR+MANUFACTURING%29+OR+%28art+OR+Art+OR+ART%29%29+AND+LANGUAGE%28English%29%29&amp;sl=541&amp;sessionSearchId=9a6079508c310b83b4cde54a2285d13f&amp;relpos=94</t>
   </si>
   <si>
@@ -1067,26 +1031,41 @@
     <t>https://www.scopus.com/record/display.uri?eid=2-s2.0-85134687980&amp;origin=resultslist&amp;sort=r-f&amp;src=s&amp;sid=9a6079508c310b83b4cde54a2285d13f&amp;sot=b&amp;sdt=cl&amp;cluster=scosubtype%2C%22ar%22%2Ct%2Bscopubstage%2C%22final%22%2Ct%2Bscolang%2C%22English%22%2Ct%2Bscosrctype%2C%22j%22%2Ct%2Bscoexactkeywords%2C%22Ethics%22%2Ct&amp;s=%28TITLE%28AI+OR+Artificial+Intelligence+OR+artificial+intelligence+OR+ARTIFICIAL+INTELLIGENCE+OR+Artificial%E2%80%90Intelligence+OR+artificial%E2%80%90intelligence+OR+ARTIFICIAL%E2%80%90INTELLIGENCE%29+AND+TITLE-ABS-KEY%28ethic*+OR+Ethic*+OR+ETHIC*%29+AND+TITLE-ABS-KEY%28%28education+OR+Education+OR+EDUCATION%29+OR+%28healthcare+OR+Healthcare+OR+HEALTHCARE%29+OR+%28transportation+OR+Transportation+OR+TRANSPORTATION%29+OR+%28finance+OR+Finance+OR+FINANCE%29+OR+%28retail+OR+Retail+OR+RETAIL%29+OR+%28manufacturing+OR+Manufacturing+OR+MANUFACTURING%29+OR+%28art+OR+Art+OR+ART%29%29+AND+LANGUAGE%28English%29%29&amp;sl=541&amp;sessionSearchId=9a6079508c310b83b4cde54a2285d13f&amp;relpos=12</t>
   </si>
   <si>
-    <t>https://www.scopus.com/record/display.uri?eid=2-s2.0-85098971645&amp;origin=resultslist&amp;sort=r-f&amp;src=s&amp;sid=9a6079508c310b83b4cde54a2285d13f&amp;sot=b&amp;sdt=cl&amp;cluster=scosubtype%2C%22ar%22%2Ct%2Bscopubstage%2C%22final%22%2Ct%2Bscolang%2C%22English%22%2Ct%2Bscosrctype%2C%22j%22%2Ct%2Bscoexactkeywords%2C%22Ethics%22%2Ct&amp;s=%28TITLE%28AI+OR+Artificial+Intelligence+OR+artificial+intelligence+OR+ARTIFICIAL+INTELLIGENCE+OR+Artificial%E2%80%90Intelligence+OR+artificial%E2%80%90intelligence+OR+ARTIFICIAL%E2%80%90INTELLIGENCE%29+AND+TITLE-ABS-KEY%28ethic*+OR+Ethic*+OR+ETHIC*%29+AND+TITLE-ABS-KEY%28%28education+OR+Education+OR+EDUCATION%29+OR+%28healthcare+OR+Healthcare+OR+HEALTHCARE%29+OR+%28transportation+OR+Transportation+OR+TRANSPORTATION%29+OR+%28finance+OR+Finance+OR+FINANCE%29+OR+%28retail+OR+Retail+OR+RETAIL%29+OR+%28manufacturing+OR+Manufacturing+OR+MANUFACTURING%29+OR+%28art+OR+Art+OR+ART%29%29+AND+LANGUAGE%28English%29%29&amp;sl=541&amp;sessionSearchId=9a6079508c310b83b4cde54a2285d13f&amp;relpos=60</t>
-  </si>
-  <si>
-    <t>https://www.scopus.com/record/display.uri?eid=2-s2.0-85090936489&amp;origin=resultslist&amp;sort=r-f&amp;src=s&amp;sid=9a6079508c310b83b4cde54a2285d13f&amp;sot=b&amp;sdt=cl&amp;cluster=scosubtype%2C%22ar%22%2Ct%2Bscopubstage%2C%22final%22%2Ct%2Bscolang%2C%22English%22%2Ct%2Bscosrctype%2C%22j%22%2Ct%2Bscoexactkeywords%2C%22Ethics%22%2Ct&amp;s=%28TITLE%28AI+OR+Artificial+Intelligence+OR+artificial+intelligence+OR+ARTIFICIAL+INTELLIGENCE+OR+Artificial%E2%80%90Intelligence+OR+artificial%E2%80%90intelligence+OR+ARTIFICIAL%E2%80%90INTELLIGENCE%29+AND+TITLE-ABS-KEY%28ethic*+OR+Ethic*+OR+ETHIC*%29+AND+TITLE-ABS-KEY%28%28education+OR+Education+OR+EDUCATION%29+OR+%28healthcare+OR+Healthcare+OR+HEALTHCARE%29+OR+%28transportation+OR+Transportation+OR+TRANSPORTATION%29+OR+%28finance+OR+Finance+OR+FINANCE%29+OR+%28retail+OR+Retail+OR+RETAIL%29+OR+%28manufacturing+OR+Manufacturing+OR+MANUFACTURING%29+OR+%28art+OR+Art+OR+ART%29%29+AND+LANGUAGE%28English%29%29&amp;sl=541&amp;sessionSearchId=9a6079508c310b83b4cde54a2285d13f&amp;relpos=43</t>
-  </si>
-  <si>
-    <t>https://www.scopus.com/record/display.uri?eid=2-s2.0-85134632305&amp;origin=resultslist&amp;sort=r-f&amp;src=s&amp;sid=9a6079508c310b83b4cde54a2285d13f&amp;sot=b&amp;sdt=cl&amp;cluster=scosubtype%2C%22ar%22%2Ct%2Bscopubstage%2C%22final%22%2Ct%2Bscolang%2C%22English%22%2Ct%2Bscosrctype%2C%22j%22%2Ct%2Bscoexactkeywords%2C%22Ethics%22%2Ct&amp;s=%28TITLE%28AI+OR+Artificial+Intelligence+OR+artificial+intelligence+OR+ARTIFICIAL+INTELLIGENCE+OR+Artificial%E2%80%90Intelligence+OR+artificial%E2%80%90intelligence+OR+ARTIFICIAL%E2%80%90INTELLIGENCE%29+AND+TITLE-ABS-KEY%28ethic*+OR+Ethic*+OR+ETHIC*%29+AND+TITLE-ABS-KEY%28%28education+OR+Education+OR+EDUCATION%29+OR+%28healthcare+OR+Healthcare+OR+HEALTHCARE%29+OR+%28transportation+OR+Transportation+OR+TRANSPORTATION%29+OR+%28finance+OR+Finance+OR+FINANCE%29+OR+%28retail+OR+Retail+OR+RETAIL%29+OR+%28manufacturing+OR+Manufacturing+OR+MANUFACTURING%29+OR+%28art+OR+Art+OR+ART%29%29+AND+LANGUAGE%28English%29%29&amp;sl=541&amp;sessionSearchId=9a6079508c310b83b4cde54a2285d13f&amp;relpos=54</t>
-  </si>
-  <si>
-    <t>https://www.scopus.com/record/display.uri?eid=2-s2.0-85141321048&amp;origin=resultslist&amp;sort=r-f&amp;src=s&amp;sid=9a6079508c310b83b4cde54a2285d13f&amp;sot=b&amp;sdt=cl&amp;cluster=scosubtype%2C%22ar%22%2Ct%2Bscopubstage%2C%22final%22%2Ct%2Bscolang%2C%22English%22%2Ct%2Bscosrctype%2C%22j%22%2Ct%2Bscoexactkeywords%2C%22Ethics%22%2Ct&amp;s=%28TITLE%28AI+OR+Artificial+Intelligence+OR+artificial+intelligence+OR+ARTIFICIAL+INTELLIGENCE+OR+Artificial%E2%80%90Intelligence+OR+artificial%E2%80%90intelligence+OR+ARTIFICIAL%E2%80%90INTELLIGENCE%29+AND+TITLE-ABS-KEY%28ethic*+OR+Ethic*+OR+ETHIC*%29+AND+TITLE-ABS-KEY%28%28education+OR+Education+OR+EDUCATION%29+OR+%28healthcare+OR+Healthcare+OR+HEALTHCARE%29+OR+%28transportation+OR+Transportation+OR+TRANSPORTATION%29+OR+%28finance+OR+Finance+OR+FINANCE%29+OR+%28retail+OR+Retail+OR+RETAIL%29+OR+%28manufacturing+OR+Manufacturing+OR+MANUFACTURING%29+OR+%28art+OR+Art+OR+ART%29%29+AND+LANGUAGE%28English%29%29&amp;sl=541&amp;sessionSearchId=9a6079508c310b83b4cde54a2285d13f&amp;relpos=11</t>
-  </si>
-  <si>
-    <t>https://www.scopus.com/record/display.uri?eid=2-s2.0-85129177393&amp;origin=resultslist&amp;sort=r-f&amp;src=s&amp;sid=9a6079508c310b83b4cde54a2285d13f&amp;sot=b&amp;sdt=cl&amp;cluster=scosubtype%2C%22ar%22%2Ct%2Bscopubstage%2C%22final%22%2Ct%2Bscolang%2C%22English%22%2Ct%2Bscosrctype%2C%22j%22%2Ct%2Bscoexactkeywords%2C%22Ethics%22%2Ct&amp;s=%28TITLE%28AI+OR+Artificial+Intelligence+OR+artificial+intelligence+OR+ARTIFICIAL+INTELLIGENCE+OR+Artificial%E2%80%90Intelligence+OR+artificial%E2%80%90intelligence+OR+ARTIFICIAL%E2%80%90INTELLIGENCE%29+AND+TITLE-ABS-KEY%28ethic*+OR+Ethic*+OR+ETHIC*%29+AND+TITLE-ABS-KEY%28%28education+OR+Education+OR+EDUCATION%29+OR+%28healthcare+OR+Healthcare+OR+HEALTHCARE%29+OR+%28transportation+OR+Transportation+OR+TRANSPORTATION%29+OR+%28finance+OR+Finance+OR+FINANCE%29+OR+%28retail+OR+Retail+OR+RETAIL%29+OR+%28manufacturing+OR+Manufacturing+OR+MANUFACTURING%29+OR+%28art+OR+Art+OR+ART%29%29+AND+LANGUAGE%28English%29%29&amp;sl=541&amp;sessionSearchId=9a6079508c310b83b4cde54a2285d13f&amp;relpos=48</t>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Title and Abstract  Relvant?</t>
+  </si>
+  <si>
+    <t>Reason if No</t>
+  </si>
+  <si>
+    <t>Not relevant to topic of study</t>
+  </si>
+  <si>
+    <t>Full Text Relevant?</t>
+  </si>
+  <si>
+    <t>Not related to research topics identified</t>
+  </si>
+  <si>
+    <t>Not relevant to topic of study after further analysis</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Full Text could not be retrieved</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1101,16 +1080,48 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -1184,19 +1195,32 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
+      <left style="thin">
         <color indexed="64"/>
-      </right>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
+      <left style="thin">
         <color indexed="64"/>
-      </right>
+      </left>
+      <right/>
       <top/>
       <bottom style="thin">
         <color indexed="64"/>
@@ -1204,18 +1228,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1225,15 +1248,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1568,8 +1605,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{772D7852-3905-4680-9C9E-A950DBEEAEAE}">
   <dimension ref="A1:D169"/>
   <sheetViews>
-    <sheetView topLeftCell="A136" workbookViewId="0">
-      <selection activeCell="A168" sqref="A168"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G164" sqref="G164"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2649,12 +2686,10 @@
       <c r="B138" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="C138" s="1" t="s">
-        <v>300</v>
-      </c>
-      <c r="D138" s="1" t="s">
-        <v>301</v>
-      </c>
+      <c r="C138" s="16" t="s">
+        <v>299</v>
+      </c>
+      <c r="D138" s="17"/>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" s="3" t="s">
@@ -2663,12 +2698,10 @@
       <c r="B139" s="5">
         <v>548</v>
       </c>
-      <c r="C139" s="3">
+      <c r="C139" s="17">
         <v>1</v>
       </c>
-      <c r="D139" s="8" t="s">
-        <v>299</v>
-      </c>
+      <c r="D139" s="19"/>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140" s="3" t="s">
@@ -2677,10 +2710,10 @@
       <c r="B140" s="3">
         <v>339</v>
       </c>
-      <c r="C140" s="3">
+      <c r="C140" s="17">
         <v>2</v>
       </c>
-      <c r="D140" s="3"/>
+      <c r="D140" s="17"/>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" s="3" t="s">
@@ -2689,12 +2722,10 @@
       <c r="B141" s="3">
         <v>187</v>
       </c>
-      <c r="C141" s="3">
+      <c r="C141" s="17">
         <v>3</v>
       </c>
-      <c r="D141" s="8" t="s">
-        <v>299</v>
-      </c>
+      <c r="D141" s="19"/>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142" s="3" t="s">
@@ -2703,10 +2734,10 @@
       <c r="B142" s="3">
         <v>133</v>
       </c>
-      <c r="C142" s="3">
+      <c r="C142" s="17">
         <v>4</v>
       </c>
-      <c r="D142" s="3"/>
+      <c r="D142" s="17"/>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143" s="3" t="s">
@@ -2715,12 +2746,10 @@
       <c r="B143" s="3">
         <v>101</v>
       </c>
-      <c r="C143" s="3">
+      <c r="C143" s="17">
         <v>5</v>
       </c>
-      <c r="D143" s="8" t="s">
-        <v>299</v>
-      </c>
+      <c r="D143" s="19"/>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144" s="3" t="s">
@@ -2729,10 +2758,10 @@
       <c r="B144" s="3">
         <v>94</v>
       </c>
-      <c r="C144" s="3">
+      <c r="C144" s="17">
         <v>6</v>
       </c>
-      <c r="D144" s="3"/>
+      <c r="D144" s="17"/>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145" s="3" t="s">
@@ -2741,12 +2770,10 @@
       <c r="B145" s="3">
         <v>92</v>
       </c>
-      <c r="C145" s="3">
+      <c r="C145" s="17">
         <v>7</v>
       </c>
-      <c r="D145" s="8" t="s">
-        <v>299</v>
-      </c>
+      <c r="D145" s="19"/>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A146" s="3" t="s">
@@ -2755,12 +2782,10 @@
       <c r="B146" s="3">
         <v>72</v>
       </c>
-      <c r="C146" s="3">
+      <c r="C146" s="17">
         <v>8</v>
       </c>
-      <c r="D146" s="8" t="s">
-        <v>299</v>
-      </c>
+      <c r="D146" s="19"/>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147" s="3" t="s">
@@ -2769,10 +2794,10 @@
       <c r="B147" s="3">
         <v>55</v>
       </c>
-      <c r="C147" s="3">
+      <c r="C147" s="17">
         <v>9</v>
       </c>
-      <c r="D147" s="3"/>
+      <c r="D147" s="17"/>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148" s="3" t="s">
@@ -2781,12 +2806,10 @@
       <c r="B148" s="3">
         <v>50</v>
       </c>
-      <c r="C148" s="3">
+      <c r="C148" s="17">
         <v>10</v>
       </c>
-      <c r="D148" s="8" t="s">
-        <v>299</v>
-      </c>
+      <c r="D148" s="19"/>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149" s="3" t="s">
@@ -2795,12 +2818,10 @@
       <c r="B149" s="3">
         <v>45</v>
       </c>
-      <c r="C149" s="3">
+      <c r="C149" s="17">
         <v>11</v>
       </c>
-      <c r="D149" s="8" t="s">
-        <v>299</v>
-      </c>
+      <c r="D149" s="19"/>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A150" s="3" t="s">
@@ -2809,10 +2830,10 @@
       <c r="B150" s="3">
         <v>42</v>
       </c>
-      <c r="C150" s="3">
+      <c r="C150" s="17">
         <v>12</v>
       </c>
-      <c r="D150" s="3"/>
+      <c r="D150" s="17"/>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A151" s="3" t="s">
@@ -2821,10 +2842,10 @@
       <c r="B151" s="3">
         <v>39</v>
       </c>
-      <c r="C151" s="3">
+      <c r="C151" s="17">
         <v>13</v>
       </c>
-      <c r="D151" s="3"/>
+      <c r="D151" s="17"/>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A152" s="3" t="s">
@@ -2833,12 +2854,10 @@
       <c r="B152" s="3">
         <v>39</v>
       </c>
-      <c r="C152" s="3">
+      <c r="C152" s="17">
         <v>14</v>
       </c>
-      <c r="D152" s="8" t="s">
-        <v>299</v>
-      </c>
+      <c r="D152" s="19"/>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A153" s="3" t="s">
@@ -2847,10 +2866,10 @@
       <c r="B153" s="3">
         <v>39</v>
       </c>
-      <c r="C153" s="3">
+      <c r="C153" s="17">
         <v>15</v>
       </c>
-      <c r="D153" s="3"/>
+      <c r="D153" s="17"/>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A154" s="3" t="s">
@@ -2859,12 +2878,10 @@
       <c r="B154" s="3">
         <v>39</v>
       </c>
-      <c r="C154" s="3">
+      <c r="C154" s="17">
         <v>16</v>
       </c>
-      <c r="D154" s="8" t="s">
-        <v>299</v>
-      </c>
+      <c r="D154" s="19"/>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A155" s="3" t="s">
@@ -2873,10 +2890,10 @@
       <c r="B155" s="3">
         <v>37</v>
       </c>
-      <c r="C155" s="3">
+      <c r="C155" s="17">
         <v>17</v>
       </c>
-      <c r="D155" s="8"/>
+      <c r="D155" s="19"/>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A156" s="3" t="s">
@@ -2885,12 +2902,10 @@
       <c r="B156" s="3">
         <v>37</v>
       </c>
-      <c r="C156" s="3">
+      <c r="C156" s="17">
         <v>18</v>
       </c>
-      <c r="D156" s="8" t="s">
-        <v>299</v>
-      </c>
+      <c r="D156" s="19"/>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A157" s="3" t="s">
@@ -2899,10 +2914,10 @@
       <c r="B157" s="3">
         <v>37</v>
       </c>
-      <c r="C157" s="3">
+      <c r="C157" s="17">
         <v>19</v>
       </c>
-      <c r="D157" s="3"/>
+      <c r="D157" s="17"/>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A158" s="3" t="s">
@@ -2911,12 +2926,10 @@
       <c r="B158" s="3">
         <v>35</v>
       </c>
-      <c r="C158" s="3">
+      <c r="C158" s="17">
         <v>20</v>
       </c>
-      <c r="D158" s="8" t="s">
-        <v>299</v>
-      </c>
+      <c r="D158" s="19"/>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A159" s="3" t="s">
@@ -2925,10 +2938,10 @@
       <c r="B159" s="3">
         <v>35</v>
       </c>
-      <c r="C159" s="3">
+      <c r="C159" s="17">
         <v>21</v>
       </c>
-      <c r="D159" s="3"/>
+      <c r="D159" s="17"/>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A160" s="3" t="s">
@@ -2937,10 +2950,10 @@
       <c r="B160" s="3">
         <v>35</v>
       </c>
-      <c r="C160" s="3">
+      <c r="C160" s="17">
         <v>22</v>
       </c>
-      <c r="D160" s="3"/>
+      <c r="D160" s="17"/>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A161" s="3" t="s">
@@ -2949,12 +2962,10 @@
       <c r="B161" s="3">
         <v>31</v>
       </c>
-      <c r="C161" s="3">
+      <c r="C161" s="17">
         <v>23</v>
       </c>
-      <c r="D161" s="8" t="s">
-        <v>299</v>
-      </c>
+      <c r="D161" s="19"/>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A162" s="3" t="s">
@@ -2963,10 +2974,10 @@
       <c r="B162" s="3">
         <v>30</v>
       </c>
-      <c r="C162" s="3">
+      <c r="C162" s="17">
         <v>24</v>
       </c>
-      <c r="D162" s="3"/>
+      <c r="D162" s="17"/>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A163" s="3" t="s">
@@ -2975,12 +2986,10 @@
       <c r="B163" s="3">
         <v>27</v>
       </c>
-      <c r="C163" s="3">
+      <c r="C163" s="17">
         <v>25</v>
       </c>
-      <c r="D163" s="8" t="s">
-        <v>299</v>
-      </c>
+      <c r="D163" s="19"/>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A164" s="3" t="s">
@@ -2989,10 +2998,10 @@
       <c r="B164" s="3">
         <v>26</v>
       </c>
-      <c r="C164" s="3">
+      <c r="C164" s="17">
         <v>26</v>
       </c>
-      <c r="D164" s="3"/>
+      <c r="D164" s="17"/>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A165" s="3" t="s">
@@ -3001,10 +3010,10 @@
       <c r="B165" s="3">
         <v>25</v>
       </c>
-      <c r="C165" s="3">
+      <c r="C165" s="17">
         <v>27</v>
       </c>
-      <c r="D165" s="3"/>
+      <c r="D165" s="17"/>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A166" s="3" t="s">
@@ -3013,10 +3022,10 @@
       <c r="B166" s="3">
         <v>24</v>
       </c>
-      <c r="C166" s="3">
+      <c r="C166" s="17">
         <v>28</v>
       </c>
-      <c r="D166" s="3"/>
+      <c r="D166" s="17"/>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A167" s="3" t="s">
@@ -3025,12 +3034,10 @@
       <c r="B167" s="3">
         <v>24</v>
       </c>
-      <c r="C167" s="3">
+      <c r="C167" s="17">
         <v>29</v>
       </c>
-      <c r="D167" s="8" t="s">
-        <v>299</v>
-      </c>
+      <c r="D167" s="19"/>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A168" s="3" t="s">
@@ -3039,12 +3046,10 @@
       <c r="B168" s="3">
         <v>23</v>
       </c>
-      <c r="C168" s="3">
+      <c r="C168" s="17">
         <v>30</v>
       </c>
-      <c r="D168" s="8" t="s">
-        <v>299</v>
-      </c>
+      <c r="D168" s="19"/>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A169" s="4" t="s">
@@ -3053,10 +3058,10 @@
       <c r="B169" s="4">
         <v>23</v>
       </c>
-      <c r="C169" s="4">
+      <c r="C169" s="18">
         <v>31</v>
       </c>
-      <c r="D169" s="4"/>
+      <c r="D169" s="17"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B130">
@@ -3068,10 +3073,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{243A80BD-AD9E-4B4B-A78E-0ABE0EBE0E01}">
-  <dimension ref="A1:H94"/>
+  <dimension ref="A1:H92"/>
   <sheetViews>
-    <sheetView topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="A86" sqref="A86:A89"/>
+    <sheetView topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="E71" sqref="E71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3627,12 +3632,10 @@
       <c r="B72" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="C72" s="1" t="s">
-        <v>300</v>
-      </c>
-      <c r="D72" s="1" t="s">
-        <v>301</v>
-      </c>
+      <c r="C72" s="16" t="s">
+        <v>299</v>
+      </c>
+      <c r="D72" s="17"/>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="5" t="s">
@@ -3641,12 +3644,10 @@
       <c r="B73" s="5">
         <v>412</v>
       </c>
-      <c r="C73" s="3">
+      <c r="C73" s="17">
         <v>1</v>
       </c>
-      <c r="D73" s="8" t="s">
-        <v>299</v>
-      </c>
+      <c r="D73" s="19"/>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="3" t="s">
@@ -3655,10 +3656,10 @@
       <c r="B74" s="3">
         <v>360</v>
       </c>
-      <c r="C74" s="3">
+      <c r="C74" s="17">
         <v>2</v>
       </c>
-      <c r="D74" s="3"/>
+      <c r="D74" s="17"/>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
@@ -3667,12 +3668,10 @@
       <c r="B75" s="3">
         <v>100</v>
       </c>
-      <c r="C75" s="3">
+      <c r="C75" s="17">
         <v>3</v>
       </c>
-      <c r="D75" s="8" t="s">
-        <v>299</v>
-      </c>
+      <c r="D75" s="19"/>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="3" t="s">
@@ -3681,12 +3680,10 @@
       <c r="B76" s="3">
         <v>79</v>
       </c>
-      <c r="C76" s="3">
+      <c r="C76" s="17">
         <v>4</v>
       </c>
-      <c r="D76" s="8" t="s">
-        <v>299</v>
-      </c>
+      <c r="D76" s="19"/>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="3" t="s">
@@ -3695,12 +3692,10 @@
       <c r="B77" s="3">
         <v>66</v>
       </c>
-      <c r="C77" s="3">
+      <c r="C77" s="17">
         <v>5</v>
       </c>
-      <c r="D77" s="8" t="s">
-        <v>299</v>
-      </c>
+      <c r="D77" s="19"/>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="3" t="s">
@@ -3709,12 +3704,10 @@
       <c r="B78" s="3">
         <v>66</v>
       </c>
-      <c r="C78" s="3">
+      <c r="C78" s="17">
         <v>6</v>
       </c>
-      <c r="D78" s="8" t="s">
-        <v>299</v>
-      </c>
+      <c r="D78" s="19"/>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="3" t="s">
@@ -3723,12 +3716,10 @@
       <c r="B79" s="3">
         <v>57</v>
       </c>
-      <c r="C79" s="3">
+      <c r="C79" s="17">
         <v>7</v>
       </c>
-      <c r="D79" s="8" t="s">
-        <v>299</v>
-      </c>
+      <c r="D79" s="19"/>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="3" t="s">
@@ -3737,12 +3728,10 @@
       <c r="B80" s="3">
         <v>52</v>
       </c>
-      <c r="C80" s="3">
+      <c r="C80" s="17">
         <v>8</v>
       </c>
-      <c r="D80" s="8" t="s">
-        <v>299</v>
-      </c>
+      <c r="D80" s="19"/>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="3" t="s">
@@ -3751,12 +3740,10 @@
       <c r="B81" s="3">
         <v>50</v>
       </c>
-      <c r="C81" s="3">
+      <c r="C81" s="17">
         <v>9</v>
       </c>
-      <c r="D81" s="8" t="s">
-        <v>299</v>
-      </c>
+      <c r="D81" s="19"/>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="3" t="s">
@@ -3765,12 +3752,10 @@
       <c r="B82" s="3">
         <v>49</v>
       </c>
-      <c r="C82" s="3">
+      <c r="C82" s="17">
         <v>10</v>
       </c>
-      <c r="D82" s="8" t="s">
-        <v>299</v>
-      </c>
+      <c r="D82" s="19"/>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="3" t="s">
@@ -3779,12 +3764,10 @@
       <c r="B83" s="3">
         <v>48</v>
       </c>
-      <c r="C83" s="3">
+      <c r="C83" s="17">
         <v>11</v>
       </c>
-      <c r="D83" s="8" t="s">
-        <v>299</v>
-      </c>
+      <c r="D83" s="19"/>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="3" t="s">
@@ -3793,12 +3776,10 @@
       <c r="B84" s="3">
         <v>45</v>
       </c>
-      <c r="C84" s="3">
+      <c r="C84" s="17">
         <v>12</v>
       </c>
-      <c r="D84" s="8" t="s">
-        <v>299</v>
-      </c>
+      <c r="D84" s="19"/>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="3" t="s">
@@ -3807,10 +3788,10 @@
       <c r="B85" s="3">
         <v>43</v>
       </c>
-      <c r="C85" s="3">
+      <c r="C85" s="17">
         <v>13</v>
       </c>
-      <c r="D85" s="3"/>
+      <c r="D85" s="17"/>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="3" t="s">
@@ -3819,12 +3800,10 @@
       <c r="B86" s="3">
         <v>40</v>
       </c>
-      <c r="C86" s="3">
+      <c r="C86" s="17">
         <v>14</v>
       </c>
-      <c r="D86" s="8" t="s">
-        <v>299</v>
-      </c>
+      <c r="D86" s="19"/>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="3" t="s">
@@ -3833,12 +3812,10 @@
       <c r="B87" s="3">
         <v>37</v>
       </c>
-      <c r="C87" s="3">
+      <c r="C87" s="17">
         <v>15</v>
       </c>
-      <c r="D87" s="8" t="s">
-        <v>299</v>
-      </c>
+      <c r="D87" s="19"/>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="3" t="s">
@@ -3847,12 +3824,10 @@
       <c r="B88" s="3">
         <v>36</v>
       </c>
-      <c r="C88" s="3">
+      <c r="C88" s="17">
         <v>16</v>
       </c>
-      <c r="D88" s="8" t="s">
-        <v>299</v>
-      </c>
+      <c r="D88" s="19"/>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="3" t="s">
@@ -3861,12 +3836,10 @@
       <c r="B89" s="3">
         <v>36</v>
       </c>
-      <c r="C89" s="3">
+      <c r="C89" s="17">
         <v>17</v>
       </c>
-      <c r="D89" s="8" t="s">
-        <v>299</v>
-      </c>
+      <c r="D89" s="19"/>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="4" t="s">
@@ -3875,26 +3848,13 @@
       <c r="B90" s="4">
         <v>35</v>
       </c>
-      <c r="C90" s="4">
+      <c r="C90" s="18">
         <v>18</v>
       </c>
-      <c r="D90" s="9"/>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C91" s="11"/>
-      <c r="D91" s="11"/>
+      <c r="D90" s="19"/>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C92" s="11"/>
-      <c r="D92" s="12"/>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C93" s="11"/>
-      <c r="D93" s="11"/>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C94" s="11"/>
-      <c r="D94" s="11"/>
+      <c r="D92" s="9"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B64">
@@ -3906,10 +3866,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB032591-C2EB-4821-9C85-5D3C30643B8C}">
-  <dimension ref="A1:E128"/>
+  <dimension ref="A1:E127"/>
   <sheetViews>
-    <sheetView topLeftCell="A93" workbookViewId="0">
-      <selection activeCell="A117" sqref="A117:A118"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4667,12 +4627,10 @@
       <c r="B97" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="C97" s="1" t="s">
-        <v>300</v>
-      </c>
-      <c r="D97" s="1" t="s">
-        <v>301</v>
-      </c>
+      <c r="C97" s="16" t="s">
+        <v>299</v>
+      </c>
+      <c r="D97" s="17"/>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="5" t="s">
@@ -4681,10 +4639,10 @@
       <c r="B98" s="5">
         <v>222</v>
       </c>
-      <c r="C98" s="3">
+      <c r="C98" s="17">
         <v>1</v>
       </c>
-      <c r="D98" s="8"/>
+      <c r="D98" s="19"/>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" s="3" t="s">
@@ -4693,12 +4651,10 @@
       <c r="B99" s="3">
         <v>202</v>
       </c>
-      <c r="C99" s="3">
+      <c r="C99" s="17">
         <v>2</v>
       </c>
-      <c r="D99" s="13" t="s">
-        <v>299</v>
-      </c>
+      <c r="D99" s="20"/>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="3" t="s">
@@ -4707,12 +4663,10 @@
       <c r="B100" s="3">
         <v>178</v>
       </c>
-      <c r="C100" s="3">
+      <c r="C100" s="17">
         <v>3</v>
       </c>
-      <c r="D100" s="13" t="s">
-        <v>299</v>
-      </c>
+      <c r="D100" s="20"/>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="3" t="s">
@@ -4721,12 +4675,10 @@
       <c r="B101" s="3">
         <v>150</v>
       </c>
-      <c r="C101" s="3">
+      <c r="C101" s="17">
         <v>4</v>
       </c>
-      <c r="D101" s="13" t="s">
-        <v>299</v>
-      </c>
+      <c r="D101" s="20"/>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" s="3" t="s">
@@ -4735,12 +4687,10 @@
       <c r="B102" s="3">
         <v>145</v>
       </c>
-      <c r="C102" s="3">
+      <c r="C102" s="17">
         <v>5</v>
       </c>
-      <c r="D102" s="13" t="s">
-        <v>299</v>
-      </c>
+      <c r="D102" s="20"/>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" s="3" t="s">
@@ -4749,12 +4699,10 @@
       <c r="B103" s="3">
         <v>104</v>
       </c>
-      <c r="C103" s="3">
+      <c r="C103" s="17">
         <v>6</v>
       </c>
-      <c r="D103" s="13" t="s">
-        <v>299</v>
-      </c>
+      <c r="D103" s="20"/>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" s="3" t="s">
@@ -4763,12 +4711,10 @@
       <c r="B104" s="3">
         <v>92</v>
       </c>
-      <c r="C104" s="3">
+      <c r="C104" s="17">
         <v>7</v>
       </c>
-      <c r="D104" s="13" t="s">
-        <v>299</v>
-      </c>
+      <c r="D104" s="20"/>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" s="3" t="s">
@@ -4777,10 +4723,10 @@
       <c r="B105" s="3">
         <v>89</v>
       </c>
-      <c r="C105" s="3">
+      <c r="C105" s="17">
         <v>8</v>
       </c>
-      <c r="D105" s="8"/>
+      <c r="D105" s="19"/>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" s="3" t="s">
@@ -4789,12 +4735,10 @@
       <c r="B106" s="3">
         <v>86</v>
       </c>
-      <c r="C106" s="3">
+      <c r="C106" s="17">
         <v>9</v>
       </c>
-      <c r="D106" s="13" t="s">
-        <v>299</v>
-      </c>
+      <c r="D106" s="20"/>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" s="3" t="s">
@@ -4803,12 +4747,10 @@
       <c r="B107" s="3">
         <v>74</v>
       </c>
-      <c r="C107" s="3">
+      <c r="C107" s="17">
         <v>10</v>
       </c>
-      <c r="D107" s="13" t="s">
-        <v>299</v>
-      </c>
+      <c r="D107" s="20"/>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" s="3" t="s">
@@ -4817,12 +4759,10 @@
       <c r="B108" s="3">
         <v>69</v>
       </c>
-      <c r="C108" s="3">
+      <c r="C108" s="17">
         <v>11</v>
       </c>
-      <c r="D108" s="13" t="s">
-        <v>299</v>
-      </c>
+      <c r="D108" s="20"/>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" s="3" t="s">
@@ -4831,10 +4771,10 @@
       <c r="B109" s="3">
         <v>64</v>
       </c>
-      <c r="C109" s="3">
+      <c r="C109" s="17">
         <v>12</v>
       </c>
-      <c r="D109" s="3"/>
+      <c r="D109" s="17"/>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" s="3" t="s">
@@ -4843,12 +4783,10 @@
       <c r="B110" s="3">
         <v>62</v>
       </c>
-      <c r="C110" s="3">
+      <c r="C110" s="17">
         <v>13</v>
       </c>
-      <c r="D110" s="13" t="s">
-        <v>299</v>
-      </c>
+      <c r="D110" s="20"/>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" s="3" t="s">
@@ -4857,10 +4795,10 @@
       <c r="B111" s="3">
         <v>56</v>
       </c>
-      <c r="C111" s="3">
+      <c r="C111" s="17">
         <v>14</v>
       </c>
-      <c r="D111" s="8"/>
+      <c r="D111" s="19"/>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" s="3" t="s">
@@ -4869,12 +4807,10 @@
       <c r="B112" s="3">
         <v>50</v>
       </c>
-      <c r="C112" s="3">
+      <c r="C112" s="17">
         <v>15</v>
       </c>
-      <c r="D112" s="13" t="s">
-        <v>299</v>
-      </c>
+      <c r="D112" s="20"/>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" s="3" t="s">
@@ -4883,12 +4819,10 @@
       <c r="B113" s="3">
         <v>40</v>
       </c>
-      <c r="C113" s="3">
+      <c r="C113" s="17">
         <v>16</v>
       </c>
-      <c r="D113" s="13" t="s">
-        <v>299</v>
-      </c>
+      <c r="D113" s="20"/>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" s="3" t="s">
@@ -4897,10 +4831,10 @@
       <c r="B114" s="3">
         <v>39</v>
       </c>
-      <c r="C114" s="3">
+      <c r="C114" s="17">
         <v>17</v>
       </c>
-      <c r="D114" s="8"/>
+      <c r="D114" s="19"/>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" s="3" t="s">
@@ -4909,12 +4843,10 @@
       <c r="B115" s="3">
         <v>36</v>
       </c>
-      <c r="C115" s="3">
+      <c r="C115" s="17">
         <v>18</v>
       </c>
-      <c r="D115" s="13" t="s">
-        <v>299</v>
-      </c>
+      <c r="D115" s="20"/>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" s="3" t="s">
@@ -4923,10 +4855,10 @@
       <c r="B116" s="3">
         <v>32</v>
       </c>
-      <c r="C116" s="3">
+      <c r="C116" s="17">
         <v>19</v>
       </c>
-      <c r="D116" s="3"/>
+      <c r="D116" s="17"/>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" s="3" t="s">
@@ -4935,12 +4867,10 @@
       <c r="B117" s="3">
         <v>30</v>
       </c>
-      <c r="C117" s="3">
+      <c r="C117" s="17">
         <v>20</v>
       </c>
-      <c r="D117" s="13" t="s">
-        <v>299</v>
-      </c>
+      <c r="D117" s="20"/>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" s="3" t="s">
@@ -4949,12 +4879,10 @@
       <c r="B118" s="3">
         <v>30</v>
       </c>
-      <c r="C118" s="3">
+      <c r="C118" s="17">
         <v>21</v>
       </c>
-      <c r="D118" s="13" t="s">
-        <v>299</v>
-      </c>
+      <c r="D118" s="20"/>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" s="4" t="s">
@@ -4963,46 +4891,22 @@
       <c r="B119" s="4">
         <v>29</v>
       </c>
-      <c r="C119" s="4">
+      <c r="C119" s="18">
         <v>22</v>
       </c>
-      <c r="D119" s="4"/>
+      <c r="D119" s="17"/>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C120" s="11"/>
-      <c r="D120" s="12"/>
-    </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C121" s="11"/>
-      <c r="D121" s="11"/>
+      <c r="D120" s="9"/>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C122" s="11"/>
-      <c r="D122" s="12"/>
-    </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C123" s="11"/>
-      <c r="D123" s="11"/>
-    </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C124" s="11"/>
-      <c r="D124" s="11"/>
-    </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C125" s="11"/>
-      <c r="D125" s="11"/>
+      <c r="D122" s="9"/>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C126" s="11"/>
-      <c r="D126" s="12"/>
+      <c r="D126" s="9"/>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C127" s="11"/>
-      <c r="D127" s="12"/>
-    </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C128" s="11"/>
-      <c r="D128" s="11"/>
+      <c r="D127" s="9"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B89">
@@ -5014,10 +4918,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAFF2C9B-1FE9-470C-9C26-7AB46B551B82}">
-  <dimension ref="A1:C52"/>
+  <dimension ref="A1:H52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C49" sqref="C49"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5025,15 +4929,18 @@
     <col min="1" max="1" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="142.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="97" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="48.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
         <v>294</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -5042,525 +4949,644 @@
       <c r="C3" s="1" t="s">
         <v>296</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="8">
+      <c r="D3" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="H3" s="13" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="6">
         <v>1</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="8">
+      <c r="C4" s="10" t="s">
+        <v>300</v>
+      </c>
+      <c r="D4" s="13"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="21" t="s">
+        <v>336</v>
+      </c>
+      <c r="H4" s="14" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="6">
         <v>2</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="8">
+      <c r="C5" s="10" t="s">
+        <v>301</v>
+      </c>
+      <c r="D5" s="13"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="21" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="6">
         <v>3</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="8">
+      <c r="C6" s="10" t="s">
+        <v>302</v>
+      </c>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="6">
         <v>4</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="8">
+      <c r="C7" s="10" t="s">
+        <v>303</v>
+      </c>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="1" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="6">
         <v>5</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="8">
+      <c r="C8" s="10" t="s">
+        <v>305</v>
+      </c>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="1" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="6">
         <v>6</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="8">
+      <c r="C9" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="6">
         <v>7</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="C10" s="3" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="8">
+      <c r="C10" s="10" t="s">
+        <v>306</v>
+      </c>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="1" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="6">
         <v>8</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="C11" s="3" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="8">
+      <c r="C11" s="10" t="s">
+        <v>307</v>
+      </c>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="1" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="6">
         <v>9</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="10" t="s">
+        <v>308</v>
+      </c>
+      <c r="D12" s="13"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="22" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="7">
+        <v>10</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>309</v>
+      </c>
+      <c r="D13" s="13"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="21" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="9"/>
+      <c r="C14" s="15"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="8" t="s">
+        <v>297</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="6">
+        <v>1</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="C16" s="12" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="8">
+      <c r="D16" s="13" t="s">
+        <v>338</v>
+      </c>
+      <c r="E16" s="13" t="s">
+        <v>338</v>
+      </c>
+      <c r="F16" s="13" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="6">
+        <v>2</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>311</v>
+      </c>
+      <c r="D17" s="13" t="s">
+        <v>338</v>
+      </c>
+      <c r="E17" s="13" t="s">
+        <v>338</v>
+      </c>
+      <c r="F17" s="13" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="6">
+        <v>3</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>312</v>
+      </c>
+      <c r="D18" s="13" t="s">
+        <v>338</v>
+      </c>
+      <c r="E18" s="13" t="s">
+        <v>338</v>
+      </c>
+      <c r="F18" s="13" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="6">
+        <v>4</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>313</v>
+      </c>
+      <c r="D19" s="13" t="s">
+        <v>338</v>
+      </c>
+      <c r="E19" s="13" t="s">
+        <v>338</v>
+      </c>
+      <c r="F19" s="13" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="6">
+        <v>5</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>314</v>
+      </c>
+      <c r="D20" s="13" t="s">
+        <v>338</v>
+      </c>
+      <c r="E20" s="13" t="s">
+        <v>338</v>
+      </c>
+      <c r="F20" s="13" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="6">
+        <v>6</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>315</v>
+      </c>
+      <c r="D21" s="13" t="s">
+        <v>338</v>
+      </c>
+      <c r="E21" s="13" t="s">
+        <v>338</v>
+      </c>
+      <c r="F21" s="13" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="6">
+        <v>7</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>316</v>
+      </c>
+      <c r="D22" s="13" t="s">
+        <v>338</v>
+      </c>
+      <c r="E22" s="13" t="s">
+        <v>338</v>
+      </c>
+      <c r="F22" s="13" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="6">
+        <v>8</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>317</v>
+      </c>
+      <c r="D23" s="13" t="s">
+        <v>338</v>
+      </c>
+      <c r="E23" s="14"/>
+      <c r="F23" s="22" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="6">
+        <v>9</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>318</v>
+      </c>
+      <c r="D24" s="13" t="s">
+        <v>338</v>
+      </c>
+      <c r="E24" s="14"/>
+      <c r="F24" s="22" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="7">
         <v>10</v>
       </c>
-      <c r="B13" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="8">
-        <v>11</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="8">
-        <v>12</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="8">
-        <v>13</v>
-      </c>
-      <c r="B16" s="3" t="s">
+      <c r="B25" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="C25" s="11" t="s">
+        <v>319</v>
+      </c>
+      <c r="D25" s="13" t="s">
+        <v>338</v>
+      </c>
+      <c r="E25" s="14"/>
+      <c r="F25" s="22" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="8" t="s">
+        <v>298</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="6">
+        <v>1</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>320</v>
+      </c>
+      <c r="D28" s="13" t="s">
+        <v>338</v>
+      </c>
+      <c r="E28" s="13" t="s">
+        <v>338</v>
+      </c>
+      <c r="F28" s="13" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="6">
+        <v>2</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="D29" s="13" t="s">
+        <v>338</v>
+      </c>
+      <c r="E29" s="13" t="s">
+        <v>338</v>
+      </c>
+      <c r="F29" s="13" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="6">
+        <v>3</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>322</v>
+      </c>
+      <c r="D30" s="13" t="s">
+        <v>338</v>
+      </c>
+      <c r="E30" s="14"/>
+      <c r="F30" s="22" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="6">
+        <v>4</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>323</v>
+      </c>
+      <c r="D31" s="13" t="s">
+        <v>338</v>
+      </c>
+      <c r="E31" s="14"/>
+      <c r="F31" s="22" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="6">
+        <v>5</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>324</v>
+      </c>
+      <c r="D32" s="13" t="s">
+        <v>338</v>
+      </c>
+      <c r="E32" s="13" t="s">
+        <v>338</v>
+      </c>
+      <c r="F32" s="13" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="6">
+        <v>6</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="D33" s="13" t="s">
+        <v>338</v>
+      </c>
+      <c r="E33" s="13" t="s">
+        <v>338</v>
+      </c>
+      <c r="F33" s="13" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="6">
+        <v>7</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="D34" s="13" t="s">
+        <v>338</v>
+      </c>
+      <c r="E34" s="14"/>
+      <c r="F34" s="22" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="6">
+        <v>8</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>327</v>
+      </c>
+      <c r="D35" s="13" t="s">
+        <v>338</v>
+      </c>
+      <c r="E35" s="14"/>
+      <c r="F35" s="22" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="6">
+        <v>9</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>263</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>328</v>
+      </c>
+      <c r="D36" s="13" t="s">
+        <v>338</v>
+      </c>
+      <c r="E36" s="13" t="s">
+        <v>338</v>
+      </c>
+      <c r="F36" s="13" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="7">
         <v>10</v>
       </c>
-      <c r="C16" s="3" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="8">
-        <v>14</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="9">
-        <v>15</v>
-      </c>
-      <c r="B18" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="10" t="s">
-        <v>297</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>295</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="8">
-        <v>1</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>177</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="8">
-        <v>2</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="8">
-        <v>3</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>180</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="8">
-        <v>4</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="8">
-        <v>5</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>193</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="8">
-        <v>6</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="8">
-        <v>7</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>178</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="8">
-        <v>8</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>190</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="8">
-        <v>9</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="8">
-        <v>10</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>185</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="8">
-        <v>11</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="8">
-        <v>12</v>
-      </c>
-      <c r="B32" s="6" t="s">
-        <v>191</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="8">
-        <v>13</v>
-      </c>
-      <c r="B33" s="6" t="s">
-        <v>173</v>
-      </c>
-      <c r="C33" s="3" t="s">
+      <c r="B37" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="C37" s="4" t="s">
         <v>329</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="8">
-        <v>14</v>
-      </c>
-      <c r="B34" s="6" t="s">
-        <v>197</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="9">
-        <v>15</v>
-      </c>
-      <c r="B35" s="7" t="s">
-        <v>198</v>
-      </c>
-      <c r="C35" s="4" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="10" t="s">
-        <v>298</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>295</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="8">
-        <v>1</v>
-      </c>
-      <c r="B38" s="3" t="s">
-        <v>285</v>
-      </c>
-      <c r="C38" s="5" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="8">
-        <v>2</v>
-      </c>
-      <c r="B39" s="3" t="s">
-        <v>279</v>
-      </c>
-      <c r="C39" s="3" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="8">
-        <v>3</v>
-      </c>
-      <c r="B40" s="3" t="s">
-        <v>211</v>
-      </c>
-      <c r="C40" s="3" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="8">
-        <v>4</v>
-      </c>
-      <c r="B41" s="3" t="s">
-        <v>209</v>
-      </c>
-      <c r="C41" s="3" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="8">
-        <v>5</v>
-      </c>
-      <c r="B42" s="3" t="s">
-        <v>216</v>
-      </c>
-      <c r="C42" s="3" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="8">
-        <v>6</v>
-      </c>
-      <c r="B43" s="3" t="s">
-        <v>241</v>
-      </c>
-      <c r="C43" s="3" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="8">
-        <v>7</v>
-      </c>
-      <c r="B44" s="3" t="s">
-        <v>235</v>
-      </c>
-      <c r="C44" s="3" t="s">
+      <c r="D37" s="13" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="8">
-        <v>8</v>
-      </c>
-      <c r="B45" s="3" t="s">
-        <v>219</v>
-      </c>
-      <c r="C45" s="3" t="s">
+      <c r="E37" s="14"/>
+      <c r="F37" s="22" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="8">
-        <v>9</v>
-      </c>
-      <c r="B46" s="3" t="s">
-        <v>263</v>
-      </c>
-      <c r="C46" s="3" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="8">
-        <v>10</v>
-      </c>
-      <c r="B47" s="3" t="s">
-        <v>213</v>
-      </c>
-      <c r="C47" s="3" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="8">
-        <v>11</v>
-      </c>
-      <c r="B48" s="3" t="s">
-        <v>253</v>
-      </c>
-      <c r="C48" s="3" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="8">
-        <v>12</v>
-      </c>
-      <c r="B49" s="3" t="s">
-        <v>239</v>
-      </c>
-      <c r="C49" s="3" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="8">
-        <v>13</v>
-      </c>
-      <c r="B50" s="3" t="s">
-        <v>248</v>
-      </c>
-      <c r="C50" s="3" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" s="8">
-        <v>14</v>
-      </c>
-      <c r="B51" s="6" t="s">
-        <v>212</v>
-      </c>
-      <c r="C51" s="3" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" s="9">
-        <v>15</v>
-      </c>
-      <c r="B52" s="7" t="s">
-        <v>243</v>
-      </c>
-      <c r="C52" s="4" t="s">
-        <v>346</v>
-      </c>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" s="9"/>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" s="9"/>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" s="9"/>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" s="9"/>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" s="9"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C9" r:id="rId1" xr:uid="{5D5D7FC3-C0AF-41BE-850B-470C4A6954A9}"/>
+    <hyperlink ref="C11" r:id="rId2" xr:uid="{E31E548A-1E17-469B-A647-6EA22BA48163}"/>
+    <hyperlink ref="C10" r:id="rId3" xr:uid="{43F0F479-31A8-4A47-8414-BCD7165FE65F}"/>
+    <hyperlink ref="C8" r:id="rId4" xr:uid="{EDDD782D-EB8B-4B42-BD6D-DA570856DF20}"/>
+    <hyperlink ref="C7" r:id="rId5" xr:uid="{82DAD324-FBF2-44EE-9464-C989FB009214}"/>
+    <hyperlink ref="C6" r:id="rId6" xr:uid="{FB2B58F5-66EF-43C2-B33B-101C32527F4A}"/>
+    <hyperlink ref="C5" r:id="rId7" xr:uid="{570DD9E4-B014-496F-8B3B-4B145A7D8E5F}"/>
+    <hyperlink ref="C4" r:id="rId8" xr:uid="{F46B1D58-55DF-459B-AB45-B5C7EC7481B5}"/>
+    <hyperlink ref="C13" r:id="rId9" xr:uid="{6F7722E2-E377-4588-9014-92BBF439E2A9}"/>
+    <hyperlink ref="C12" r:id="rId10" xr:uid="{EA32ED5D-CAFE-49B9-BCF9-A8A903671244}"/>
+    <hyperlink ref="C17" r:id="rId11" xr:uid="{12CD1494-EC2E-4784-871B-946EC4949342}"/>
+    <hyperlink ref="C16" r:id="rId12" xr:uid="{22D00E92-0F62-4CFD-943E-C24172AD6BF7}"/>
+    <hyperlink ref="C18" r:id="rId13" xr:uid="{A4DCE397-B66A-473B-B4E1-0556105A71C6}"/>
+    <hyperlink ref="C20" r:id="rId14" xr:uid="{C631989C-947C-44A4-A7EB-08BB90EF2323}"/>
+    <hyperlink ref="C19" r:id="rId15" xr:uid="{45BA9E90-AB70-4435-B398-977FE34FEC53}"/>
+    <hyperlink ref="C21" r:id="rId16" xr:uid="{62C15964-9420-456F-81E6-D96F41F8443D}"/>
+    <hyperlink ref="C22" r:id="rId17" xr:uid="{EAB387D6-A6E3-40F6-8E1D-3E24B7BF61A9}"/>
+    <hyperlink ref="C23" r:id="rId18" xr:uid="{5C8B2E78-F806-4A56-AE14-903719405838}"/>
+    <hyperlink ref="C25" r:id="rId19" xr:uid="{B821CC35-E3FD-4AA6-B884-F68999AE12C9}"/>
+    <hyperlink ref="C24" r:id="rId20" xr:uid="{ADD9D1F9-F5A8-4080-8017-3BC4C33262B9}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>